<commit_message>
added doc for process flow
</commit_message>
<xml_diff>
--- a/doc/特征工程设计说明.xlsx
+++ b/doc/特征工程设计说明.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{129FB156-956C-4C02-997D-5803EE717DD0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E3E82DE-C1C9-416E-B1AB-1743E4700EE5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7812" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8928" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="15" r:id="rId1"/>
+    <sheet name="架构设计" sheetId="15" r:id="rId1"/>
+    <sheet name="流程设计" sheetId="16" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -6189,6 +6190,2896 @@
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
           <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215228</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50608</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>594758</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>134686</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0747C04-CEBD-423D-9CB7-70EE73F2A740}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3471046" y="5814099"/>
+          <a:ext cx="2208330" cy="804514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>数据字典</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Var_10</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>字段 生成自 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Y</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>模块 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Z</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>字段，分子是</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>，分母是</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>2 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>。。。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>45967</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215228</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>92647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{740A8206-06BE-483B-ADE3-7F571E4D83AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="121" idx="3"/>
+          <a:endCxn id="21" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2989117" y="5269131"/>
+          <a:ext cx="481929" cy="947225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215229</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>81286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>594759</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>171299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Rectangle 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCB94FB6-424A-475B-801A-7460B206730B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3471047" y="6745322"/>
+          <a:ext cx="2208330" cy="810450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>百分比变量数据文件</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>                         Var_10</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  Var_11 .....</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>客户</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>月份          </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>0.8</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>         0.9</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>45967</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215229</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>126292</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A147BFF-0D3A-4FF5-829B-4428985AC86B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="121" idx="3"/>
+          <a:endCxn id="23" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2989117" y="5269131"/>
+          <a:ext cx="481930" cy="1881416"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215229</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>5085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>594759</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>89163</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Rectangle 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03646E1A-C839-4301-BC90-FDC232A10244}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3471047" y="7749776"/>
+          <a:ext cx="2208330" cy="804514"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>统计变量数据文件</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>                         Var_20</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  Var_21 .....</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>客户                 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>0.8</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>         0.9</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>45967</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215229</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>47124</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA41FFCA-620B-41A3-9820-53348314EE1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="121" idx="3"/>
+          <a:endCxn id="25" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2989117" y="5269131"/>
+          <a:ext cx="481930" cy="2882902"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>302722</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>340822</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Rectangle 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{750ED1B7-839F-4A42-9B26-F21A770B60A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4775662" y="2491740"/>
+          <a:ext cx="1866900" cy="815339"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>实时生产 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ff_online_production</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>通过数据字典配置，调用特征工程生成衍生变量</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>413744</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158673</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>368730</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>67491</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rectangle 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D790F89-A5A9-486A-86A6-3E66DCE9BB60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4277084" y="3663873"/>
+          <a:ext cx="2393386" cy="785118"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>数据字典（从离线分析生成的数据字典中做筛选）</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Var_10</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>字段 生成自 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Y</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>模块 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Z</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>字段，分子是</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>，分母是</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>。。。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>391237</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>16972</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158673</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7A05ABC-26EA-46C8-B6F1-E4D1E75802E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="51" idx="0"/>
+          <a:endCxn id="49" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5473777" y="3307079"/>
+          <a:ext cx="235335" cy="356794"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>597847</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>156670</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371104</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>98030</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rectangle 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0002F90A-5C3B-4ABE-9BF7-ED10405039A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1415265" y="2498088"/>
+          <a:ext cx="2821257" cy="1022015"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>文件：</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4_ff_online_production var_generate.py</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>（</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>示例在线生产变量生成入口</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>函数</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>）</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>将</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>JSON</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>文件解包，并以合适格式送给流程函数调用</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371104</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>302722</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{887A2F8A-5944-4A75-BD05-A94B1EC6D631}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="53" idx="3"/>
+          <a:endCxn id="49" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4234444" y="2899410"/>
+          <a:ext cx="541218" cy="32100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104899</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166254</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55419</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Rectangle 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1AC40A1-E45F-481E-B423-F612F5E67DB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1531917" y="1427018"/>
+          <a:ext cx="2388920" cy="577042"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Python Server</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>80159</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>179676</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>156670</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Straight Arrow Connector 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B9C2BF-300F-4E17-9CCD-367CBCCAD21C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="53" idx="0"/>
+          <a:endCxn id="55" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2726377" y="2004060"/>
+          <a:ext cx="99517" cy="494028"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>79168</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>176052</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>13855</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>69274</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Rectangle 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75CAFCD-6770-4E4E-9CC8-F6AF00203E52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1506186" y="356161"/>
+          <a:ext cx="2373087" cy="613658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>客户端调用</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>46512</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>69274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>80159</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>166254</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Arrow Connector 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66D5F5C4-E36E-4FE3-9108-AC626FBC8C59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="55" idx="0"/>
+          <a:endCxn id="57" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2692730" y="969819"/>
+          <a:ext cx="33647" cy="457199"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>391237</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>67491</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>594758</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>92647</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Connector: Curved 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A207B23-55D1-4B07-A887-D660390DEA53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="21" idx="3"/>
+          <a:endCxn id="51" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="5473777" y="4448991"/>
+          <a:ext cx="203521" cy="1602496"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector4">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -112323"/>
+            <a:gd name="adj2" fmla="val 62248"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>22662</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="121" name="Rectangle 120">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A3309C4-4CDD-4EA4-9255-6999DF219FAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1122217" y="4932218"/>
+          <a:ext cx="1866900" cy="673826"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>离线分析 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ff_offline_analysis</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>358141</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>601981</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="130" name="Rectangle 129">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3793E0-5C20-41DF-84F5-B908FAA5E34A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6050281" y="693420"/>
+          <a:ext cx="2682240" cy="1590403"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>文件：</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ff_funcs </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>（</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="zh-CN" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>基本函数</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>）</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>数据检查（月份出现字符串、数值分布）</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>百分比衍生</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>基础统计</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>时间段对比</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>连续出现</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>增加</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>分区统计</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>字符统计</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>340822</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>480061</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="131" name="Straight Arrow Connector 130">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{318CF795-0F75-46FC-8532-3946A251B65F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="49" idx="3"/>
+          <a:endCxn id="130" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6642562" y="2283823"/>
+          <a:ext cx="748839" cy="615587"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>253329</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>23259</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>49379</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="139" name="Rectangle 138">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D32C3E6-5E9D-48B9-8F3E-1A28FC3CA1A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7164669" y="3639826"/>
+          <a:ext cx="2208330" cy="791053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>中间衍生变量数据集</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>480061</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>5443</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>138294</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="140" name="Straight Arrow Connector 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35699910-E927-4186-ADCF-EF0D7A53FAC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="130" idx="2"/>
+          <a:endCxn id="139" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7391401" y="2283823"/>
+          <a:ext cx="877433" cy="1356003"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>531322</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="151" name="Rectangle 150">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBAF8AB2-87EE-4E36-B25E-0FFD7931ACF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8661862" y="2506980"/>
+          <a:ext cx="2402378" cy="861059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>组合变量 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ff_conbination_vars</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>对于特殊逻辑、不能抽象为特征工程的变量，使用</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>python</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>代码自定义变量</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>138294</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>531322</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>134626</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="152" name="Straight Arrow Connector 151">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DFBE7B8-67EE-4E2C-8A24-98A881DA020D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="139" idx="0"/>
+          <a:endCxn id="151" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8268834" y="2937510"/>
+          <a:ext cx="393028" cy="702316"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>573369</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>157486</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>343299</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>72239</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="177" name="Rectangle 176">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86A9B79F-6E9E-4B6D-849F-77B690C1CA14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10532709" y="3662686"/>
+          <a:ext cx="2208330" cy="791053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>最终输出衍生变量数据集</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>458334</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>157486</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="178" name="Straight Arrow Connector 177">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50DA7CBE-74F8-4D17-9755-B428BBE896A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="151" idx="3"/>
+          <a:endCxn id="177" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11064240" y="2937510"/>
+          <a:ext cx="572634" cy="725176"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
@@ -6477,7 +9368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533258F0-2C73-49C5-ABF9-FFD88CDA7F28}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AK25" sqref="AK25"/>
     </sheetView>
   </sheetViews>
@@ -6490,4 +9381,20 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A225B683-5392-4ED1-AEC5-F5938D6ADE31}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
doc update: offline analysis process
</commit_message>
<xml_diff>
--- a/doc/特征工程设计说明.xlsx
+++ b/doc/特征工程设计说明.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E3E82DE-C1C9-416E-B1AB-1743E4700EE5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EA714AC9-0722-434C-9F9E-42403EB34D33}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8928" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10044" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="架构设计" sheetId="15" r:id="rId1"/>
-    <sheet name="流程设计" sheetId="16" r:id="rId2"/>
+    <sheet name="在线生成流程设计" sheetId="16" r:id="rId2"/>
+    <sheet name="离线分析流程设计" sheetId="17" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -6845,15 +6846,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>302722</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>243087</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>157370</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>340822</xdr:colOff>
+      <xdr:colOff>281187</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>139147</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6868,8 +6869,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4775662" y="2491740"/>
-          <a:ext cx="1866900" cy="815339"/>
+          <a:off x="3900687" y="2396987"/>
+          <a:ext cx="1866900" cy="843169"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6943,16 +6944,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>413744</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>158673</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19878</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118917</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>368730</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>67491</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490331</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>27735</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6967,8 +6968,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4277084" y="3663873"/>
-          <a:ext cx="2393386" cy="785118"/>
+          <a:off x="3677478" y="3736760"/>
+          <a:ext cx="3518453" cy="770210"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7149,15 +7150,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>391237</xdr:colOff>
+      <xdr:colOff>566937</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>139147</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>16972</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>158673</xdr:rowOff>
+      <xdr:colOff>559905</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>118917</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7174,9 +7175,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5473777" y="3307079"/>
-          <a:ext cx="235335" cy="356794"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4834137" y="3240156"/>
+          <a:ext cx="602568" cy="496604"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7204,16 +7205,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>597847</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>21378</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>156670</xdr:rowOff>
+      <xdr:rowOff>77157</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>371104</xdr:colOff>
+      <xdr:colOff>404235</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>98030</xdr:rowOff>
+      <xdr:rowOff>99391</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7228,8 +7229,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1415265" y="2498088"/>
-          <a:ext cx="2821257" cy="1022015"/>
+          <a:off x="630978" y="2316774"/>
+          <a:ext cx="2821257" cy="1055904"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7537,15 +7538,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>371104</xdr:colOff>
+      <xdr:colOff>404235</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>62120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>302722</xdr:colOff>
+      <xdr:colOff>243087</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>127350</xdr:rowOff>
+      <xdr:rowOff>88274</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7563,8 +7564,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4234444" y="2899410"/>
-          <a:ext cx="541218" cy="32100"/>
+          <a:off x="3452235" y="2818572"/>
+          <a:ext cx="448452" cy="26154"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7694,9 +7695,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>179676</xdr:colOff>
+      <xdr:colOff>212807</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>156670</xdr:rowOff>
+      <xdr:rowOff>77157</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7714,8 +7715,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2726377" y="2004060"/>
-          <a:ext cx="99517" cy="494028"/>
+          <a:off x="1908959" y="1917921"/>
+          <a:ext cx="132648" cy="398853"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7911,13 +7912,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>391237</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>67491</xdr:rowOff>
+      <xdr:colOff>594758</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>27735</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>594758</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>559905</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>92647</xdr:rowOff>
     </xdr:to>
@@ -7936,15 +7937,12 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="5473777" y="4448991"/>
-          <a:ext cx="203521" cy="1602496"/>
+        <a:xfrm flipV="1">
+          <a:off x="4861958" y="4506970"/>
+          <a:ext cx="574747" cy="1443138"/>
         </a:xfrm>
-        <a:prstGeom prst="curvedConnector4">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -112323"/>
-            <a:gd name="adj2" fmla="val 62248"/>
-          </a:avLst>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
         </a:prstGeom>
         <a:ln w="28575">
           <a:solidFill>
@@ -8060,14 +8058,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>358141</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>35118</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>601981</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>5443</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>45199</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8082,8 +8080,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6050281" y="693420"/>
-          <a:ext cx="2682240" cy="1590403"/>
+          <a:off x="5234941" y="379675"/>
+          <a:ext cx="2682240" cy="1560585"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8608,15 +8606,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>340822</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>5443</xdr:rowOff>
+      <xdr:colOff>281187</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>45199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>480061</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>62120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8634,8 +8632,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6642562" y="2283823"/>
-          <a:ext cx="748839" cy="615587"/>
+          <a:off x="5767587" y="1940260"/>
+          <a:ext cx="808474" cy="878312"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8664,93 +8662,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>253329</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>134626</xdr:rowOff>
+      <xdr:colOff>480061</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>45199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>23259</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>49379</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="139" name="Rectangle 138">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D32C3E6-5E9D-48B9-8F3E-1A28FC3CA1A0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7164669" y="3639826"/>
-          <a:ext cx="2208330" cy="791053"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>中间衍生变量数据集</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>480061</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>5443</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>138294</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>458334</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>134626</xdr:rowOff>
+      <xdr:rowOff>157486</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8763,13 +8683,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="130" idx="2"/>
-          <a:endCxn id="139" idx="0"/>
+          <a:endCxn id="177" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7391401" y="2283823"/>
-          <a:ext cx="877433" cy="1356003"/>
+          <a:off x="6576061" y="1940260"/>
+          <a:ext cx="4245473" cy="1662791"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8797,16 +8717,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>531322</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1235</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>20211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>574813</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4969</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8821,8 +8741,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8661862" y="2506980"/>
-          <a:ext cx="2402378" cy="861059"/>
+          <a:off x="8535635" y="881602"/>
+          <a:ext cx="2402378" cy="846150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8912,16 +8832,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>138294</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>281187</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>98729</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>531322</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>134626</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1235</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>62120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8933,14 +8853,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="139" idx="0"/>
+          <a:stCxn id="49" idx="3"/>
           <a:endCxn id="151" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8268834" y="2937510"/>
-          <a:ext cx="393028" cy="702316"/>
+          <a:off x="5767587" y="1304677"/>
+          <a:ext cx="2768048" cy="1513895"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9046,10 +8966,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>592824</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>4969</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
@@ -9067,14 +8987,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="151" idx="3"/>
+          <a:stCxn id="151" idx="2"/>
           <a:endCxn id="177" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11064240" y="2937510"/>
-          <a:ext cx="572634" cy="725176"/>
+          <a:off x="9736824" y="1727752"/>
+          <a:ext cx="1084710" cy="1875299"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -9098,6 +9018,1781 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>112642</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>136456</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>106017</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53009</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rectangle 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BE44A3E-3577-4B30-B917-FB5E4423B01B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="722242" y="3582021"/>
+          <a:ext cx="2431775" cy="950223"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>配置文件</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="900" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="900" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>工作流步骤</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="900" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="900" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>JsonPath -&gt; DataFrame(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="900" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>数据集</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="900" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="900" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>数据字典名</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="900" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>109330</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>212807</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>136456</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{263449D1-6FE0-4CE0-99CC-DECA7BA56657}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="29" idx="0"/>
+          <a:endCxn id="53" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1938130" y="3372678"/>
+          <a:ext cx="103477" cy="209343"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>271054</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>166551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40984</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>72102</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F1B9F97-5861-4270-A480-D6DFFD828167}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4538254" y="863237"/>
+          <a:ext cx="2208330" cy="776408"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>N</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>个月的百分比变量</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>日期</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>501450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>3523</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7770852-0A61-4C6A-94D7-376D897A3711}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7437120" y="1501140"/>
+          <a:ext cx="2208330" cy="780763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>第</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>N</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>个月的汇总</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>509070</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>163543</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{892782CF-3E3D-4486-8E71-5B829AE2E066}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7444740" y="2362200"/>
+          <a:ext cx="2208330" cy="780763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>第</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>N-1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>个月的汇总</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>501450</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>155923</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68516277-58A8-451E-80AB-70C30E298EE8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7437120" y="3230880"/>
+          <a:ext cx="2208330" cy="780763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>......</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Right Brace 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5749A214-0B77-4A1B-B5EE-691A663F4ADF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9799320" y="1447800"/>
+          <a:ext cx="396240" cy="3055620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>509070</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133063</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44FFC714-3FAE-443A-898E-B063C7947B84}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10492740" y="2682240"/>
+          <a:ext cx="2208330" cy="780763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>共计</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>N</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>个月的汇总</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>90351</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>469881</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57951</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25583C1E-68C2-4A1C-8601-1E26257C2519}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1919151" y="849086"/>
+          <a:ext cx="2208330" cy="776408"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>源文件</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>469881</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>18090</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>271054</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>32241</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{796A6F17-9F1C-4058-9ABA-743A5E33D4D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="3"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4127481" y="1237290"/>
+          <a:ext cx="410773" cy="14151"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40984</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>32241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>138378</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05F0427C-C2E9-46C5-BFFF-B182A12D197B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6746584" y="1251441"/>
+          <a:ext cx="690536" cy="628651"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40984</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>32241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>123682</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14199640-ADFA-4E0C-9A6D-99A150D04824}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6746584" y="1251441"/>
+          <a:ext cx="698156" cy="1484812"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40984</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>32241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>116061</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6612DF6-AE9E-4A14-803A-AD8949DBA5C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="5" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6746584" y="1251441"/>
+          <a:ext cx="690536" cy="2348049"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>501450</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>11143</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rectangle 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53499515-4169-48D9-9A8B-20A539CA8023}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7437120" y="4137660"/>
+          <a:ext cx="2208330" cy="780763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>第</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>M</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>个月的汇总</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40984</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>32241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>145997</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE280C04-55BE-46C2-9F68-CF7C334F9CFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="27" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6746584" y="1251441"/>
+          <a:ext cx="690536" cy="3248842"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>249283</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>31568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19213</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>111291</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="43" name="Rectangle 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D01D1D4C-B01F-4A76-9CC6-AD9C291C3286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11831683" y="1773282"/>
+          <a:ext cx="2208330" cy="776409"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>共计</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>N</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>个月的百分比</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>+</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>汇总变量</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>40984</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>32241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>134248</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>31568</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Connector: Curved 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23BD15E8-7762-4123-95B6-1EEC434ADFF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="43" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4917784" y="1251441"/>
+          <a:ext cx="8018064" cy="521841"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>509070</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>111291</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>134248</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>93202</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Connector: Curved 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A34C9D54-78F3-48FB-B4AB-000C177F77EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="3"/>
+          <a:endCxn id="43" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10872270" y="2549691"/>
+          <a:ext cx="2063578" cy="504425"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>446315</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>32656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>484415</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rectangle 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{325026AC-5F9C-4574-9A46-C27D4D3587FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15076715" y="1774370"/>
+          <a:ext cx="1866900" cy="858077"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>二次衍生、三次衍生。。。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19213</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>71430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>446315</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>113352</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="Straight Arrow Connector 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E396D1E5-86D0-4AF0-B73D-B2D3685DD833}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="43" idx="3"/>
+          <a:endCxn id="51" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14040013" y="2161487"/>
+          <a:ext cx="1036702" cy="41922"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>478972</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>250371</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>87087</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Rectangle 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47B01093-5080-4C23-9842-E51E3F65C680}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1698172" y="1817914"/>
+          <a:ext cx="990599" cy="359230"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>百分比衍生</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>174172</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>87086</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>119744</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Rectangle 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EFEDF2A-31C7-4133-AC45-F23C27AF8F80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4441372" y="2198914"/>
+          <a:ext cx="1132114" cy="359230"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>统计变量衍生</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>141515</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>10885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>54429</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>21773</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Rectangle 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52FEF487-A3F8-4F25-BF1A-687FFCB2C79C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11114315" y="1055914"/>
+          <a:ext cx="1132114" cy="359230"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>合并数据集</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -9368,7 +11063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533258F0-2C73-49C5-ABF9-FFD88CDA7F28}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AK25" sqref="AK25"/>
     </sheetView>
   </sheetViews>
@@ -9387,8 +11082,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A225B683-5392-4ED1-AEC5-F5938D6ADE31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA629FA-759B-450D-8B8E-7812C76C2E5D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
moved entrance py to root dir added base month in all production entrance py
</commit_message>
<xml_diff>
--- a/doc/特征工程设计说明.xlsx
+++ b/doc/特征工程设计说明.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{95AC4DD6-7647-49FA-B007-3530EE81F35A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7CDB8676-1514-417A-9F81-7006B344658B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12276" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13392" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="架构设计" sheetId="15" r:id="rId1"/>
-    <sheet name="在线生成流程设计" sheetId="16" r:id="rId2"/>
+    <sheet name="在线生产流程设计" sheetId="16" r:id="rId2"/>
     <sheet name="离线分析流程设计" sheetId="17" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -997,13 +997,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>183969</xdr:colOff>
+      <xdr:colOff>183968</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>22861</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>222069</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>65313</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
@@ -1020,8 +1020,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6889569" y="2809604"/>
-          <a:ext cx="1866900" cy="673826"/>
+          <a:off x="5267597" y="2809604"/>
+          <a:ext cx="2319745" cy="673826"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1067,7 +1067,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>ff_offline_analysis</a:t>
+            <a:t>ff_main_offline_analysis_rolling.py</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
             <a:solidFill>
@@ -1081,8 +1081,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>507819</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>124641</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>140426</xdr:rowOff>
     </xdr:from>
@@ -1108,8 +1108,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6201048" y="1882140"/>
-          <a:ext cx="3059429" cy="927464"/>
+          <a:off x="6427470" y="1882140"/>
+          <a:ext cx="2833007" cy="927464"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1266,10 +1266,10 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>544287</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>124641</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>10885</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
@@ -1288,12 +1288,13 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="34" idx="0"/>
+          <a:endCxn id="24" idx="2"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7859487" y="3494314"/>
-          <a:ext cx="349398" cy="396176"/>
+          <a:off x="6427470" y="3483430"/>
+          <a:ext cx="159444" cy="407060"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1426,27 +1427,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>1_ff_data_check.py</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
+            <a:t>ff_data_check.py</a:t>
+          </a:r>
           <a:r>
             <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
@@ -1806,7 +1788,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6649314" y="5069095"/>
+          <a:off x="5027343" y="5069095"/>
           <a:ext cx="2821257" cy="992328"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1887,7 +1869,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>2_ff_offline_analysis var_generate.py</a:t>
+            <a:t>ff_offline_analysis_var_generate_rolling.py</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1997,8 +1979,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>507819</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>124641</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
@@ -2024,8 +2006,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="7823019" y="3483430"/>
-          <a:ext cx="236924" cy="1585665"/>
+          <a:off x="6427470" y="3483430"/>
+          <a:ext cx="10502" cy="1585665"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2296,7 +2278,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>ff_offline_production</a:t>
+            <a:t>ff_main_offline_production.py</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
             <a:solidFill>
@@ -2613,8 +2595,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>222069</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>65313</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>11431</xdr:rowOff>
     </xdr:from>
@@ -2640,8 +2622,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8756469" y="3146517"/>
-          <a:ext cx="1129231" cy="1437873"/>
+          <a:off x="7587342" y="3146517"/>
+          <a:ext cx="676387" cy="1437873"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2822,8 +2804,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>222069</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>65313</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>11431</xdr:rowOff>
     </xdr:from>
@@ -2849,8 +2831,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8756469" y="3146517"/>
-          <a:ext cx="1129231" cy="2450244"/>
+          <a:off x="7587342" y="3146517"/>
+          <a:ext cx="676387" cy="2450244"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3015,8 +2997,8 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>222069</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>65313</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>11431</xdr:rowOff>
     </xdr:from>
@@ -3042,8 +3024,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8756469" y="3146517"/>
-          <a:ext cx="1129231" cy="3419073"/>
+          <a:off x="7587342" y="3146517"/>
+          <a:ext cx="676387" cy="3419073"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3990,7 +3972,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3_ff_offline_production var_generate.py</a:t>
+            <a:t>ff_offline_production_var_generate.py</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5138,7 +5120,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>ff_online_production</a:t>
+            <a:t>ff_main_online_production.py</a:t>
           </a:r>
           <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1000">
             <a:solidFill>
@@ -5574,7 +5556,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>4_ff_online_production var_generate.py</a:t>
+            <a:t>ff_online_production_var_generate.py</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5945,6 +5927,108 @@
             </a:rPr>
             <a:t>Python Server</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ff_server.py</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -6236,6 +6320,285 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>43543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>32658</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Callout: Bent Line with Accent Bar 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9676871A-03AC-49AC-B4DC-C0BEA09A3C71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13030200" y="7707086"/>
+          <a:ext cx="4288972" cy="1730829"/>
+        </a:xfrm>
+        <a:prstGeom prst="accentCallout2">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 18750"/>
+            <a:gd name="adj2" fmla="val -8333"/>
+            <a:gd name="adj3" fmla="val 18750"/>
+            <a:gd name="adj4" fmla="val -16667"/>
+            <a:gd name="adj5" fmla="val -103224"/>
+            <a:gd name="adj6" fmla="val -58089"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="2000" b="1"/>
+            <a:t>调度工具或者最外层，需要生成</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2000" b="1"/>
+            <a:t>base month</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="2000" b="1"/>
+            <a:t>，供内层的每个函数使用</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>65313</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>54427</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Oval 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2A7F19E-6AF6-4994-B9FA-8414114D7231}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10069286" y="5116284"/>
+          <a:ext cx="4876800" cy="1034143"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>119742</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>326571</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>108856</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Oval 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAB4AFEA-D421-424D-A088-6880AC18B229}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17602200" y="6738256"/>
+          <a:ext cx="4876800" cy="1034143"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>43543</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>131581</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>431162</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Connector 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8124BFB6-365E-4A9A-9DC2-4415F38BE0A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="0"/>
+          <a:endCxn id="72" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="17319172" y="7620952"/>
+          <a:ext cx="997219" cy="951549"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7225,13 +7588,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>21378</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>77157</xdr:rowOff>
+      <xdr:rowOff>77156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>404235</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>99391</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7246,8 +7609,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="630978" y="2316774"/>
-          <a:ext cx="2821257" cy="1055904"/>
+          <a:off x="630978" y="2355536"/>
+          <a:ext cx="2821257" cy="1210623"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7432,12 +7795,79 @@
             </a:rPr>
             <a:t>文件解包，读取工作流步骤，根据配置文件中所需解析配置，调用实时生产流程</a:t>
           </a:r>
+          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uLnTx/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>需指定</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>base month</a:t>
+          </a:r>
           <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uLnTx/>
@@ -7462,7 +7892,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>243086</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>88274</xdr:rowOff>
+      <xdr:rowOff>156688</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7481,7 +7911,7 @@
       <xdr:spPr>
         <a:xfrm flipV="1">
           <a:off x="3452235" y="2864789"/>
-          <a:ext cx="448451" cy="27645"/>
+          <a:ext cx="448451" cy="96059"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -7613,7 +8043,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>212807</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>77157</xdr:rowOff>
+      <xdr:rowOff>77156</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -7631,8 +8061,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1908959" y="1917921"/>
-          <a:ext cx="132648" cy="398853"/>
+          <a:off x="1908959" y="1950720"/>
+          <a:ext cx="132648" cy="404816"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8830,14 +9260,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>112642</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>136456</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>22156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>106017</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>53009</xdr:rowOff>
+      <xdr:rowOff>113969</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8852,8 +9282,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="722242" y="3582021"/>
-          <a:ext cx="2431775" cy="950223"/>
+          <a:off x="722242" y="3702616"/>
+          <a:ext cx="2431775" cy="968113"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9008,14 +9438,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>109330</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>99391</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>212807</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>136456</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>22156</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9033,8 +9463,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1938130" y="3372678"/>
-          <a:ext cx="103477" cy="209343"/>
+          <a:off x="1938130" y="3566159"/>
+          <a:ext cx="103477" cy="136457"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -12970,8 +13400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533258F0-2C73-49C5-ABF9-FFD88CDA7F28}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK25" sqref="AK25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -12989,8 +13419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A225B683-5392-4ED1-AEC5-F5938D6ADE31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated doc, changed online production main filename
</commit_message>
<xml_diff>
--- a/doc/特征工程设计说明.xlsx
+++ b/doc/特征工程设计说明.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7CDB8676-1514-417A-9F81-7006B344658B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E89F702E-525D-4CCF-8E7A-E2BB6548CA7A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13392" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14508" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="824" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="架构设计" sheetId="15" r:id="rId1"/>
@@ -6599,6 +6599,167 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>67429</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>124032</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>402774</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>7683</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Rectangle 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35514FF2-3C34-4D43-93D2-5BD919059E14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22219858" y="5523346"/>
+          <a:ext cx="2164145" cy="754508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>在线生产调度配置文件</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>步骤</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ID  JSONPATH  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1000">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>对应的数据字典</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>10886</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165945</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>67429</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152943</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Straight Arrow Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58F33A5E-A111-4B4B-B40C-9FCF871202C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="1"/>
+          <a:endCxn id="97" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="21553715" y="5565259"/>
+          <a:ext cx="666143" cy="335341"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7304,7 +7465,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>ff_online_production_var_generate.py</a:t>
+            <a:t>ff_main_online_production.py</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -7659,7 +7820,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -7673,58 +7834,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>文件：</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:uLnTx/>
-              <a:uFillTx/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>ff_server</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:endParaRPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1100" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uLnTx/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
+            <a:t>ff_online_production_var_generate.py</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
@@ -7940,15 +8051,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>104899</xdr:colOff>
+      <xdr:colOff>120139</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>166254</xdr:rowOff>
+      <xdr:rowOff>128154</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>55419</xdr:colOff>
+      <xdr:colOff>70659</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7963,8 +8074,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1531917" y="1427018"/>
-          <a:ext cx="2388920" cy="577042"/>
+          <a:off x="729739" y="1354974"/>
+          <a:ext cx="2388920" cy="610986"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8011,7 +8122,7 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="2000" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
               <a:ln>
                 <a:noFill/>
               </a:ln>
@@ -8026,6 +8137,59 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
             <a:t>Python Server</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="zh-CN" altLang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>文件：</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ff_server</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -8035,9 +8199,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>80159</xdr:colOff>
+      <xdr:colOff>95399</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
@@ -8061,8 +8225,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="1908959" y="1950720"/>
-          <a:ext cx="132648" cy="404816"/>
+          <a:off x="1924199" y="1965960"/>
+          <a:ext cx="117408" cy="389576"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8207,9 +8371,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>80159</xdr:colOff>
+      <xdr:colOff>95399</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>166254</xdr:rowOff>
+      <xdr:rowOff>128154</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -8227,8 +8391,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2692730" y="969819"/>
-          <a:ext cx="33647" cy="457199"/>
+          <a:off x="1875312" y="945574"/>
+          <a:ext cx="48887" cy="409400"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -13400,8 +13564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533258F0-2C73-49C5-ABF9-FFD88CDA7F28}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -13419,8 +13583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A225B683-5392-4ED1-AEC5-F5938D6ADE31}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>